<commit_message>
update presentaion and data analysis
</commit_message>
<xml_diff>
--- a/data/Data analysis.xlsx
+++ b/data/Data analysis.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="120" windowWidth="20520" windowHeight="10875"/>
+    <workbookView xWindow="0" yWindow="180" windowWidth="20520" windowHeight="10815"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="3" r:id="rId1"/>
@@ -123,7 +123,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -137,10 +137,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -172,6 +175,10 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -285,91 +292,11 @@
           <c:xVal>
             <c:numRef>
               <c:f>main!$D$15:$D$26</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>200</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>210</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>220</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>230</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>240</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>250</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>260</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>270</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>280</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>290</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>300</c:v>
-                </c:pt>
-              </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
               <c:f>main!$E$15:$E$26</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>82</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>75</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>61</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>52</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>5</c:v>
-                </c:pt>
-              </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
@@ -401,85 +328,11 @@
           <c:xVal>
             <c:numRef>
               <c:f>main!$D$27:$D$38</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>200</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>210</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>220</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>240</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>250</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>260</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>270</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>280</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>290</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>300</c:v>
-                </c:pt>
-              </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
               <c:f>main!$E$27:$E$38</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>79</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>72</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>56</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>43</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>6</c:v>
-                </c:pt>
-              </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
@@ -493,91 +346,11 @@
           <c:xVal>
             <c:numRef>
               <c:f>main!$D$39:$D$50</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>200</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>210</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>220</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>230</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>240</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>250</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>260</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>270</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>280</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>290</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>300</c:v>
-                </c:pt>
-              </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
               <c:f>main!$E$39:$E$50</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>58</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>55</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>39</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>36</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
@@ -591,91 +364,11 @@
           <c:xVal>
             <c:numRef>
               <c:f>main!$D$51:$D$62</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>200</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>210</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>220</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>230</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>240</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>250</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>260</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>270</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>280</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>290</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>300</c:v>
-                </c:pt>
-              </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
               <c:f>main!$E$51:$E$62</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>76</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>63</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>58</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>55</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>46</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>3</c:v>
-                </c:pt>
-              </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
@@ -688,11 +381,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="74989952"/>
-        <c:axId val="74975872"/>
+        <c:axId val="65772928"/>
+        <c:axId val="65791104"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="74989952"/>
+        <c:axId val="65772928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -702,12 +395,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="74975872"/>
+        <c:crossAx val="65791104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="74975872"/>
+        <c:axId val="65791104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -718,7 +411,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="74989952"/>
+        <c:crossAx val="65772928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -770,7 +463,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -802,11 +494,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="98006528"/>
-        <c:axId val="98299904"/>
+        <c:axId val="127120128"/>
+        <c:axId val="127122048"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="98006528"/>
+        <c:axId val="127120128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -833,19 +525,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98299904"/>
+        <c:crossAx val="127122048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="98299904"/>
+        <c:axId val="127122048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -868,21 +559,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98006528"/>
+        <c:crossAx val="127120128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -969,11 +658,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="100382592"/>
-        <c:axId val="100397824"/>
+        <c:axId val="127147008"/>
+        <c:axId val="127149184"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="100382592"/>
+        <c:axId val="127147008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -995,19 +684,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100397824"/>
+        <c:crossAx val="127149184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="100397824"/>
+        <c:axId val="127149184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1030,21 +718,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100382592"/>
+        <c:crossAx val="127147008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1150,7 +836,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1182,11 +867,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="101629952"/>
-        <c:axId val="101631872"/>
+        <c:axId val="127170048"/>
+        <c:axId val="127171968"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="101629952"/>
+        <c:axId val="127170048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1208,19 +893,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101631872"/>
+        <c:crossAx val="127171968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="101631872"/>
+        <c:axId val="127171968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1243,21 +927,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101629952"/>
+        <c:crossAx val="127170048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1359,7 +1041,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1391,11 +1072,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="102579584"/>
-        <c:axId val="102655488"/>
+        <c:axId val="130699264"/>
+        <c:axId val="130701184"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="102579584"/>
+        <c:axId val="130699264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1422,19 +1103,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102655488"/>
+        <c:crossAx val="130701184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="102655488"/>
+        <c:axId val="130701184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1457,21 +1137,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102579584"/>
+        <c:crossAx val="130699264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1561,11 +1239,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="109649280"/>
-        <c:axId val="109709184"/>
+        <c:axId val="130722048"/>
+        <c:axId val="130724224"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="109649280"/>
+        <c:axId val="130722048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1587,19 +1265,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109709184"/>
+        <c:crossAx val="130724224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="109709184"/>
+        <c:axId val="130724224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1622,21 +1299,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109649280"/>
+        <c:crossAx val="130722048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1666,6 +1341,10 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -1733,37 +1412,37 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.3510805500982316E-2</c:v>
+                  <c:v>1.1408644400785855E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.5849514563106793E-2</c:v>
+                  <c:v>1.9441747572815533E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.7004854368932045E-2</c:v>
+                  <c:v>2.0597087378640775E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.10976415094339623</c:v>
+                  <c:v>3.9009433962264153E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.12883707865168539</c:v>
+                  <c:v>4.9249063670411986E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.19461754068716094</c:v>
+                  <c:v>7.481645569620253E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.19513513513513514</c:v>
+                  <c:v>7.1261261261261255E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.21559090909090908</c:v>
+                  <c:v>7.9672905525846702E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.27913874345549738</c:v>
+                  <c:v>0.1198891797556719</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.29570547945205483</c:v>
+                  <c:v>0.1159109589041096</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.30712139219015278</c:v>
+                  <c:v>0.11824193548387096</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1779,91 +1458,11 @@
           <c:xVal>
             <c:numRef>
               <c:f>main!$D$15:$D$26</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>200</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>210</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>220</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>230</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>240</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>250</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>260</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>270</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>280</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>290</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>300</c:v>
-                </c:pt>
-              </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
               <c:f>main!$H$15:$H$26</c:f>
-              <c:numCache>
-                <c:formatCode>0.000%</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6.8399613899613895E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>9.35E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.14460853432282003</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.17301094890510949</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.19740540540540541</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.25306521739130433</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.28071331058020477</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.30181506849315065</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.29939393939393938</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.29965092748735245</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.29984285714285713</c:v>
-                </c:pt>
-              </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
@@ -1877,85 +1476,11 @@
           <c:xVal>
             <c:numRef>
               <c:f>main!$D$27:$D$38</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>200</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>210</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>220</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>240</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>250</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>260</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>270</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>280</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>290</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>300</c:v>
-                </c:pt>
-              </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
               <c:f>main!$H$27:$H$38</c:f>
-              <c:numCache>
-                <c:formatCode>0.000%</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3.7823529411764707E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>8.0124760076775423E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.11129545454545453</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.16936029411764708</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.20202782764811489</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.28990575916230366</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.27382960413080892</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.29832203389830508</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.28640034071550252</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.30101515151515151</c:v>
-                </c:pt>
-              </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
@@ -1969,91 +1494,11 @@
           <c:xVal>
             <c:numRef>
               <c:f>main!$D$39:$D$50</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>200</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>210</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>220</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>230</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>240</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>250</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>260</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>270</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>280</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>290</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>300</c:v>
-                </c:pt>
-              </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
               <c:f>main!$H$39:$H$50</c:f>
-              <c:numCache>
-                <c:formatCode>0.000%</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.11313207547169811</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.15134132841328413</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.1628394495412844</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.22932085561497326</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.25926595744680853</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.27252577319587629</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.31623857868020305</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.29194915254237286</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.3067020202020202</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.30924369747899161</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.31197913188647747</c:v>
-                </c:pt>
-              </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
@@ -2067,91 +1512,11 @@
           <c:xVal>
             <c:numRef>
               <c:f>main!$D$51:$D$62</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>200</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>210</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>220</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>230</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>240</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>250</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>260</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>270</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>280</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>290</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>300</c:v>
-                </c:pt>
-              </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
               <c:f>main!$H$51:$H$62</c:f>
-              <c:numCache>
-                <c:formatCode>0.000%</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8.8053435114503822E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.13382402234636873</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.15246494464944649</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.16425229357798166</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.19642057761732851</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.28426315789473683</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.26991237113402061</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.28110750853242322</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.29846458684654298</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.29297457627118645</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.31558040201005028</c:v>
-                </c:pt>
-              </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
@@ -2164,11 +1529,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="102290176"/>
-        <c:axId val="102291712"/>
+        <c:axId val="108216320"/>
+        <c:axId val="108217856"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="102290176"/>
+        <c:axId val="108216320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2178,12 +1543,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102291712"/>
+        <c:crossAx val="108217856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="102291712"/>
+        <c:axId val="108217856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2194,7 +1559,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102290176"/>
+        <c:crossAx val="108216320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2307,7 +1672,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2339,11 +1703,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="43993344"/>
-        <c:axId val="44454272"/>
+        <c:axId val="108262912"/>
+        <c:axId val="108264832"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="43993344"/>
+        <c:axId val="108262912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2365,19 +1729,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44454272"/>
+        <c:crossAx val="108264832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="44454272"/>
+        <c:axId val="108264832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2400,21 +1763,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="43993344"/>
+        <c:crossAx val="108262912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2459,7 +1820,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2641,11 +2001,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="48267648"/>
-        <c:axId val="48269952"/>
+        <c:axId val="65914368"/>
+        <c:axId val="65916288"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="48267648"/>
+        <c:axId val="65914368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2672,19 +2032,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48269952"/>
+        <c:crossAx val="65916288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="48269952"/>
+        <c:axId val="65916288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2707,21 +2066,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48267648"/>
+        <c:crossAx val="65914368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2958,11 +2315,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="50385280"/>
-        <c:axId val="50387584"/>
+        <c:axId val="126893056"/>
+        <c:axId val="126915712"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="50385280"/>
+        <c:axId val="126893056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2984,19 +2341,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50387584"/>
+        <c:crossAx val="126915712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="50387584"/>
+        <c:axId val="126915712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3019,21 +2375,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50385280"/>
+        <c:crossAx val="126893056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3133,7 +2487,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3315,11 +2668,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="50993792"/>
-        <c:axId val="51000064"/>
+        <c:axId val="130553344"/>
+        <c:axId val="130555264"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="50993792"/>
+        <c:axId val="130553344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3341,19 +2694,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51000064"/>
+        <c:crossAx val="130555264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="51000064"/>
+        <c:axId val="130555264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3376,21 +2728,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50993792"/>
+        <c:crossAx val="130553344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3486,7 +2836,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3668,11 +3017,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="51174784"/>
-        <c:axId val="52012160"/>
+        <c:axId val="130577536"/>
+        <c:axId val="130579456"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="51174784"/>
+        <c:axId val="130577536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3699,19 +3048,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="52012160"/>
+        <c:crossAx val="130579456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="52012160"/>
+        <c:axId val="130579456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3734,21 +3082,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51174784"/>
+        <c:crossAx val="130577536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3985,11 +3331,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="57477376"/>
-        <c:axId val="60667008"/>
+        <c:axId val="130630784"/>
+        <c:axId val="130632704"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="57477376"/>
+        <c:axId val="130630784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4011,19 +3357,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="60667008"/>
+        <c:crossAx val="130632704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="60667008"/>
+        <c:axId val="130632704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4046,21 +3391,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57477376"/>
+        <c:crossAx val="130630784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4160,7 +3503,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -4365,11 +3707,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="79218560"/>
-        <c:axId val="79220736"/>
+        <c:axId val="130668416"/>
+        <c:axId val="127074304"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="79218560"/>
+        <c:axId val="130668416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4391,19 +3733,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="79220736"/>
+        <c:crossAx val="127074304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="79220736"/>
+        <c:axId val="127074304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4426,21 +3767,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="79218560"/>
+        <c:crossAx val="130668416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5447,7 +4786,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -5457,37 +4796,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
+      <selection activeCell="A50" sqref="A15:XFD50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" customWidth="1"/>
     <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" customWidth="1"/>
     <col min="6" max="6" width="17.7109375" style="5" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="12"/>
+    <col min="7" max="7" width="12.85546875" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+    </row>
+    <row r="2" spans="1:9" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
         <v>10</v>
       </c>
       <c r="B2" t="s">
@@ -5505,7 +4844,7 @@
       <c r="F2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="11" t="s">
         <v>7</v>
       </c>
     </row>
@@ -5528,7 +4867,7 @@
       <c r="F3" s="5">
         <v>0</v>
       </c>
-      <c r="H3" s="12">
+      <c r="H3" s="11">
         <v>0</v>
       </c>
     </row>
@@ -5551,9 +4890,9 @@
       <c r="F4" s="5">
         <v>4.0000000000000002E-4</v>
       </c>
-      <c r="H4" s="12">
-        <f t="shared" ref="H4:H62" si="0">(F4*E4*8*A3+(100-E4)*30/96*96)/(E4*8*A3+(100-E4)*96)</f>
-        <v>3.3510805500982316E-2</v>
+      <c r="H4" s="11">
+        <f>(F4*E4*8*A3+(100-E4)*10/96*96)/(E4*8*A3+(100-E4)*96)</f>
+        <v>1.1408644400785855E-2</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -5575,9 +4914,9 @@
       <c r="F5" s="5">
         <v>1.5E-3</v>
       </c>
-      <c r="H5" s="12">
-        <f t="shared" si="0"/>
-        <v>5.5849514563106793E-2</v>
+      <c r="H5" s="11">
+        <f>(F5*E5*8*A4+(100-E5)*10/96*96)/(E5*8*A4+(100-E5)*96)</f>
+        <v>1.9441747572815533E-2</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -5599,9 +4938,9 @@
       <c r="F6" s="5">
         <v>2.8999999999999998E-3</v>
       </c>
-      <c r="H6" s="12">
-        <f t="shared" si="0"/>
-        <v>5.7004854368932045E-2</v>
+      <c r="H6" s="11">
+        <f t="shared" ref="H6:H32" si="0">(F6*E6*8*A5+(100-E6)*10/96*96)/(E6*8*A5+(100-E6)*96)</f>
+        <v>2.0597087378640775E-2</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -5623,9 +4962,9 @@
       <c r="F7" s="5">
         <v>5.4999999999999997E-3</v>
       </c>
-      <c r="H7" s="12">
+      <c r="H7" s="11">
         <f t="shared" si="0"/>
-        <v>0.10976415094339623</v>
+        <v>3.9009433962264153E-2</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -5647,9 +4986,9 @@
       <c r="F8" s="5">
         <v>1.5299999999999999E-2</v>
       </c>
-      <c r="H8" s="12">
+      <c r="H8" s="11">
         <f t="shared" si="0"/>
-        <v>0.12883707865168539</v>
+        <v>4.9249063670411986E-2</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -5671,9 +5010,9 @@
       <c r="F9" s="5">
         <v>3.5099999999999999E-2</v>
       </c>
-      <c r="H9" s="12">
+      <c r="H9" s="11">
         <f t="shared" si="0"/>
-        <v>0.19461754068716094</v>
+        <v>7.481645569620253E-2</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -5695,9 +5034,9 @@
       <c r="F10" s="5">
         <v>2.3E-2</v>
       </c>
-      <c r="H10" s="12">
+      <c r="H10" s="11">
         <f t="shared" si="0"/>
-        <v>0.19513513513513514</v>
+        <v>7.1261261261261255E-2</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -5719,9 +5058,9 @@
       <c r="F11" s="5">
         <v>3.3700000000000001E-2</v>
       </c>
-      <c r="H11" s="12">
+      <c r="H11" s="11">
         <f t="shared" si="0"/>
-        <v>0.21559090909090908</v>
+        <v>7.9672905525846702E-2</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -5743,9 +5082,9 @@
       <c r="F12" s="5">
         <v>0.1709</v>
       </c>
-      <c r="H12" s="12">
+      <c r="H12" s="11">
         <f t="shared" si="0"/>
-        <v>0.27913874345549738</v>
+        <v>0.1198891797556719</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -5767,9 +5106,9 @@
       <c r="F13" s="5">
         <v>0.18990000000000001</v>
       </c>
-      <c r="H13" s="12">
+      <c r="H13" s="11">
         <f t="shared" si="0"/>
-        <v>0.29570547945205483</v>
+        <v>0.1159109589041096</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -5791,12 +5130,12 @@
       <c r="F14" s="5">
         <v>0.25490000000000002</v>
       </c>
-      <c r="H14" s="12">
+      <c r="H14" s="11">
         <f t="shared" si="0"/>
-        <v>0.30712139219015278</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.11824193548387096</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>10</v>
       </c>
@@ -5815,300 +5154,300 @@
       <c r="F15" s="5">
         <v>0</v>
       </c>
-      <c r="H15" s="12">
+      <c r="H15" s="11">
+        <f>(F15*E15*8*A14+(100-E15)*10/96*96)/(E15*8*A14+(100-E15)*96)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>10</v>
+      </c>
+      <c r="B16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16">
+        <v>100</v>
+      </c>
+      <c r="D16">
+        <v>200</v>
+      </c>
+      <c r="E16">
+        <v>82</v>
+      </c>
+      <c r="F16" s="5">
+        <v>4.1000000000000003E-3</v>
+      </c>
+      <c r="H16" s="11">
+        <f t="shared" si="0"/>
+        <v>2.4963320463320466E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>10</v>
+      </c>
+      <c r="B17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17">
+        <v>100</v>
+      </c>
+      <c r="D17">
+        <v>210</v>
+      </c>
+      <c r="E17">
+        <v>75</v>
+      </c>
+      <c r="F17" s="5">
+        <v>5.8999999999999999E-3</v>
+      </c>
+      <c r="H17" s="11">
+        <f t="shared" si="0"/>
+        <v>3.3976190476190472E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>10</v>
+      </c>
+      <c r="B18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18">
+        <v>100</v>
+      </c>
+      <c r="D18">
+        <v>220</v>
+      </c>
+      <c r="E18">
+        <v>61</v>
+      </c>
+      <c r="F18" s="5">
+        <v>1.5800000000000002E-2</v>
+      </c>
+      <c r="H18" s="11">
+        <f t="shared" si="0"/>
+        <v>5.4163265306122456E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>10</v>
+      </c>
+      <c r="B19" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19">
+        <v>100</v>
+      </c>
+      <c r="D19">
+        <v>230</v>
+      </c>
+      <c r="E19">
+        <v>52</v>
+      </c>
+      <c r="F19" s="5">
+        <v>1.8499999999999999E-2</v>
+      </c>
+      <c r="H19" s="11">
+        <f t="shared" si="0"/>
+        <v>6.3521897810218983E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>10</v>
+      </c>
+      <c r="B20" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20">
+        <v>100</v>
+      </c>
+      <c r="D20">
+        <v>240</v>
+      </c>
+      <c r="E20">
+        <v>45</v>
+      </c>
+      <c r="F20" s="5">
+        <v>2.86E-2</v>
+      </c>
+      <c r="H20" s="11">
+        <f t="shared" si="0"/>
+        <v>7.3531531531531538E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>10</v>
+      </c>
+      <c r="B21" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21">
+        <v>100</v>
+      </c>
+      <c r="D21">
+        <v>250</v>
+      </c>
+      <c r="E21">
+        <v>25</v>
+      </c>
+      <c r="F21" s="5">
+        <v>3.9100000000000003E-2</v>
+      </c>
+      <c r="H21" s="11">
+        <f t="shared" si="0"/>
+        <v>9.0021739130434791E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>10</v>
+      </c>
+      <c r="B22" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22">
+        <v>100</v>
+      </c>
+      <c r="D22">
+        <v>260</v>
+      </c>
+      <c r="E22">
+        <v>14</v>
+      </c>
+      <c r="F22" s="5">
+        <v>4.6399999999999997E-2</v>
+      </c>
+      <c r="H22" s="11">
+        <f t="shared" si="0"/>
+        <v>9.7266211604095557E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>10</v>
+      </c>
+      <c r="B23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23">
+        <v>100</v>
+      </c>
+      <c r="D23">
+        <v>270</v>
+      </c>
+      <c r="E23">
+        <v>16</v>
+      </c>
+      <c r="F23" s="5">
+        <v>0.23449999999999999</v>
+      </c>
+      <c r="H23" s="11">
+        <f>(F23*E23*8*A22+(100-E23)*10/96*96)/(E23*8*A22+(100-E23)*96)</f>
+        <v>0.12202054794520546</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>10</v>
+      </c>
+      <c r="B24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24">
+        <v>100</v>
+      </c>
+      <c r="D24">
+        <v>280</v>
+      </c>
+      <c r="E24">
+        <v>6</v>
+      </c>
+      <c r="F24" s="5">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="H24" s="11">
+        <f t="shared" si="0"/>
+        <v>0.10158249158249159</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>10</v>
+      </c>
+      <c r="B25" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25">
+        <v>100</v>
+      </c>
+      <c r="D25">
+        <v>290</v>
+      </c>
+      <c r="E25">
+        <v>7</v>
+      </c>
+      <c r="F25" s="5">
+        <v>9.4799999999999995E-2</v>
+      </c>
+      <c r="H25" s="11">
+        <f t="shared" si="0"/>
+        <v>0.10361382799325464</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>10</v>
+      </c>
+      <c r="B26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26">
+        <v>100</v>
+      </c>
+      <c r="D26">
+        <v>300</v>
+      </c>
+      <c r="E26">
+        <v>5</v>
+      </c>
+      <c r="F26" s="5">
+        <v>1.1259999999999999E-2</v>
+      </c>
+      <c r="H26" s="11">
+        <f t="shared" si="0"/>
+        <v>0.10026302521008404</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>10</v>
+      </c>
+      <c r="B27" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27">
+        <v>130</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>100</v>
+      </c>
+      <c r="F27" s="5">
+        <v>0</v>
+      </c>
+      <c r="H27" s="11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>10</v>
-      </c>
-      <c r="B16" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16">
-        <v>100</v>
-      </c>
-      <c r="D16">
-        <v>200</v>
-      </c>
-      <c r="E16">
-        <v>82</v>
-      </c>
-      <c r="F16" s="5">
-        <v>4.1000000000000003E-3</v>
-      </c>
-      <c r="H16" s="12">
-        <f t="shared" si="0"/>
-        <v>6.8399613899613895E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>10</v>
-      </c>
-      <c r="B17" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17">
-        <v>100</v>
-      </c>
-      <c r="D17">
-        <v>210</v>
-      </c>
-      <c r="E17">
-        <v>75</v>
-      </c>
-      <c r="F17" s="5">
-        <v>5.8999999999999999E-3</v>
-      </c>
-      <c r="H17" s="12">
-        <f t="shared" si="0"/>
-        <v>9.35E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>10</v>
-      </c>
-      <c r="B18" t="s">
-        <v>12</v>
-      </c>
-      <c r="C18">
-        <v>100</v>
-      </c>
-      <c r="D18">
-        <v>220</v>
-      </c>
-      <c r="E18">
-        <v>61</v>
-      </c>
-      <c r="F18" s="5">
-        <v>1.5800000000000002E-2</v>
-      </c>
-      <c r="H18" s="12">
-        <f t="shared" si="0"/>
-        <v>0.14460853432282003</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>10</v>
-      </c>
-      <c r="B19" t="s">
-        <v>12</v>
-      </c>
-      <c r="C19">
-        <v>100</v>
-      </c>
-      <c r="D19">
-        <v>230</v>
-      </c>
-      <c r="E19">
-        <v>52</v>
-      </c>
-      <c r="F19" s="5">
-        <v>1.8499999999999999E-2</v>
-      </c>
-      <c r="H19" s="12">
-        <f t="shared" si="0"/>
-        <v>0.17301094890510949</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>10</v>
-      </c>
-      <c r="B20" t="s">
-        <v>12</v>
-      </c>
-      <c r="C20">
-        <v>100</v>
-      </c>
-      <c r="D20">
-        <v>240</v>
-      </c>
-      <c r="E20">
-        <v>45</v>
-      </c>
-      <c r="F20" s="5">
-        <v>2.86E-2</v>
-      </c>
-      <c r="H20" s="12">
-        <f t="shared" si="0"/>
-        <v>0.19740540540540541</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>10</v>
-      </c>
-      <c r="B21" t="s">
-        <v>12</v>
-      </c>
-      <c r="C21">
-        <v>100</v>
-      </c>
-      <c r="D21">
-        <v>250</v>
-      </c>
-      <c r="E21">
-        <v>25</v>
-      </c>
-      <c r="F21" s="5">
-        <v>3.9100000000000003E-2</v>
-      </c>
-      <c r="H21" s="12">
-        <f t="shared" si="0"/>
-        <v>0.25306521739130433</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>10</v>
-      </c>
-      <c r="B22" t="s">
-        <v>12</v>
-      </c>
-      <c r="C22">
-        <v>100</v>
-      </c>
-      <c r="D22">
-        <v>260</v>
-      </c>
-      <c r="E22">
-        <v>14</v>
-      </c>
-      <c r="F22" s="5">
-        <v>4.6399999999999997E-2</v>
-      </c>
-      <c r="H22" s="12">
-        <f t="shared" si="0"/>
-        <v>0.28071331058020477</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>10</v>
-      </c>
-      <c r="B23" t="s">
-        <v>12</v>
-      </c>
-      <c r="C23">
-        <v>100</v>
-      </c>
-      <c r="D23">
-        <v>270</v>
-      </c>
-      <c r="E23">
-        <v>16</v>
-      </c>
-      <c r="F23" s="5">
-        <v>0.23449999999999999</v>
-      </c>
-      <c r="H23" s="12">
-        <f t="shared" si="0"/>
-        <v>0.30181506849315065</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>10</v>
-      </c>
-      <c r="B24" t="s">
-        <v>12</v>
-      </c>
-      <c r="C24">
-        <v>100</v>
-      </c>
-      <c r="D24">
-        <v>280</v>
-      </c>
-      <c r="E24">
-        <v>6</v>
-      </c>
-      <c r="F24" s="5">
-        <v>5.2999999999999999E-2</v>
-      </c>
-      <c r="H24" s="12">
-        <f t="shared" si="0"/>
-        <v>0.29939393939393938</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>10</v>
-      </c>
-      <c r="B25" t="s">
-        <v>12</v>
-      </c>
-      <c r="C25">
-        <v>100</v>
-      </c>
-      <c r="D25">
-        <v>290</v>
-      </c>
-      <c r="E25">
-        <v>7</v>
-      </c>
-      <c r="F25" s="5">
-        <v>9.4799999999999995E-2</v>
-      </c>
-      <c r="H25" s="12">
-        <f t="shared" si="0"/>
-        <v>0.29965092748735245</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>10</v>
-      </c>
-      <c r="B26" t="s">
-        <v>12</v>
-      </c>
-      <c r="C26">
-        <v>100</v>
-      </c>
-      <c r="D26">
-        <v>300</v>
-      </c>
-      <c r="E26">
-        <v>5</v>
-      </c>
-      <c r="F26" s="5">
-        <v>1.1259999999999999E-2</v>
-      </c>
-      <c r="H26" s="12">
-        <f t="shared" si="0"/>
-        <v>0.29984285714285713</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>10</v>
-      </c>
-      <c r="B27" t="s">
-        <v>12</v>
-      </c>
-      <c r="C27">
-        <v>130</v>
-      </c>
-      <c r="D27">
-        <v>0</v>
-      </c>
-      <c r="E27">
-        <v>100</v>
-      </c>
-      <c r="F27" s="5">
-        <v>0</v>
-      </c>
-      <c r="H27" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>10</v>
       </c>
@@ -6127,12 +5466,12 @@
       <c r="F28" s="5">
         <v>1.1999999999999999E-3</v>
       </c>
-      <c r="H28" s="12">
+      <c r="H28" s="11">
         <f t="shared" si="0"/>
-        <v>3.7823529411764707E-2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1.3313725490196078E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>10</v>
       </c>
@@ -6151,12 +5490,12 @@
       <c r="F29" s="5">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="H29" s="12">
+      <c r="H29" s="11">
         <f t="shared" si="0"/>
-        <v>8.0124760076775423E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2.9740882917466412E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>10</v>
       </c>
@@ -6175,9 +5514,9 @@
       <c r="F30" s="5">
         <v>1.7399999999999999E-2</v>
       </c>
-      <c r="H30" s="12">
+      <c r="H30" s="11">
         <f t="shared" si="0"/>
-        <v>0.11129545454545453</v>
+        <v>4.5007575757575753E-2</v>
       </c>
     </row>
     <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -6199,12 +5538,12 @@
       <c r="F31" s="5">
         <v>0.21440000000000001</v>
       </c>
-      <c r="H31" s="12">
+      <c r="H31" s="11">
         <f t="shared" si="0"/>
         <v>0.21440000000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>10</v>
       </c>
@@ -6223,12 +5562,12 @@
       <c r="F32" s="5">
         <v>3.44E-2</v>
       </c>
-      <c r="H32" s="12">
+      <c r="H32" s="11">
         <f t="shared" si="0"/>
-        <v>0.16936029411764708</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+        <v>6.8257352941176477E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>10</v>
       </c>
@@ -6247,12 +5586,12 @@
       <c r="F33" s="5">
         <v>2.63E-2</v>
       </c>
-      <c r="H33" s="12">
-        <f t="shared" si="0"/>
-        <v>0.20202782764811489</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H33" s="11">
+        <f>(F33*E33*8*A32+(100-E33)*10/96*96)/(E33*8*A32+(100-E33)*96)</f>
+        <v>7.4110412926391381E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>10</v>
       </c>
@@ -6271,12 +5610,12 @@
       <c r="F34" s="5">
         <v>0.21659999999999999</v>
       </c>
-      <c r="H34" s="12">
-        <f t="shared" si="0"/>
-        <v>0.28990575916230366</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H34" s="11">
+        <f>(F34*E34*8*A33+(100-E34)*10/96*96)/(E34*8*A33+(100-E34)*96)</f>
+        <v>0.1306561954624782</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>10</v>
       </c>
@@ -6295,12 +5634,12 @@
       <c r="F35" s="5">
         <v>7.5999999999999998E-2</v>
       </c>
-      <c r="H35" s="12">
-        <f t="shared" si="0"/>
-        <v>0.27382960413080892</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H35" s="11">
+        <f t="shared" ref="H35:H39" si="1">(F35*E35*8*A34+(100-E35)*10/96*96)/(E35*8*A34+(100-E35)*96)</f>
+        <v>9.9561101549053357E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>10</v>
       </c>
@@ -6319,12 +5658,12 @@
       <c r="F36" s="5">
         <v>0.1452</v>
       </c>
-      <c r="H36" s="12">
-        <f t="shared" si="0"/>
-        <v>0.29832203389830508</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H36" s="11">
+        <f t="shared" si="1"/>
+        <v>0.10764406779661016</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>10</v>
       </c>
@@ -6343,12 +5682,12 @@
       <c r="F37" s="5">
         <v>7.6799999999999993E-2</v>
       </c>
-      <c r="H37" s="12">
-        <f t="shared" si="0"/>
-        <v>0.28640034071550252</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H37" s="11">
+        <f t="shared" si="1"/>
+        <v>0.10113628620102214</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>10</v>
       </c>
@@ -6367,12 +5706,12 @@
       <c r="F38" s="5">
         <v>8.5099999999999995E-2</v>
       </c>
-      <c r="H38" s="12">
-        <f t="shared" si="0"/>
-        <v>0.30101515151515151</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H38" s="11">
+        <f t="shared" si="1"/>
+        <v>0.1032037037037037</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>10</v>
       </c>
@@ -6391,12 +5730,12 @@
       <c r="F39" s="5">
         <v>0</v>
       </c>
-      <c r="H39" s="12">
-        <f t="shared" si="0"/>
+      <c r="H39" s="11">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>10</v>
       </c>
@@ -6415,12 +5754,12 @@
       <c r="F40" s="5">
         <v>1.06E-2</v>
       </c>
-      <c r="H40" s="12">
-        <f t="shared" si="0"/>
-        <v>0.11313207547169811</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H40" s="11">
+        <f>(F40*E40*8*A39+(100-E40)*10/96*96)/(E40*8*A39+(100-E40)*96)</f>
+        <v>4.2377358490566036E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>10</v>
       </c>
@@ -6439,12 +5778,12 @@
       <c r="F41" s="5">
         <v>1.1299999999999999E-2</v>
       </c>
-      <c r="H41" s="12">
-        <f t="shared" si="0"/>
-        <v>0.15134132841328413</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H41" s="11">
+        <f t="shared" ref="H41:H49" si="2">(F41*E41*8*A40+(100-E41)*10/96*96)/(E41*8*A40+(100-E41)*96)</f>
+        <v>5.4477859778597787E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>10</v>
       </c>
@@ -6463,12 +5802,12 @@
       <c r="F42" s="5">
         <v>1.5900000000000001E-2</v>
       </c>
-      <c r="H42" s="12">
-        <f t="shared" si="0"/>
-        <v>0.1628394495412844</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H42" s="11">
+        <f t="shared" si="2"/>
+        <v>5.9628440366972478E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>10</v>
       </c>
@@ -6487,12 +5826,12 @@
       <c r="F43" s="5">
         <v>7.3200000000000001E-2</v>
       </c>
-      <c r="H43" s="12">
-        <f t="shared" si="0"/>
-        <v>0.22932085561497326</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H43" s="11">
+        <f t="shared" si="2"/>
+        <v>9.3402852049910876E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>10</v>
       </c>
@@ -6511,12 +5850,12 @@
       <c r="F44" s="5">
         <v>0.1457</v>
       </c>
-      <c r="H44" s="12">
-        <f t="shared" si="0"/>
-        <v>0.25926595744680853</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H44" s="11">
+        <f t="shared" si="2"/>
+        <v>0.11742198581560284</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>10</v>
       </c>
@@ -6535,12 +5874,12 @@
       <c r="F45" s="5">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="H45" s="12">
-        <f t="shared" si="0"/>
-        <v>0.27252577319587629</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H45" s="11">
+        <f t="shared" si="2"/>
+        <v>9.6408934707903779E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>10</v>
       </c>
@@ -6559,12 +5898,12 @@
       <c r="F46" s="5">
         <v>0.36159999999999998</v>
       </c>
-      <c r="H46" s="12">
-        <f t="shared" si="0"/>
-        <v>0.31623857868020305</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H46" s="11">
+        <f t="shared" si="2"/>
+        <v>0.12376818950930625</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>10</v>
       </c>
@@ -6583,12 +5922,12 @@
       <c r="F47" s="5">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="H47" s="12">
-        <f t="shared" si="0"/>
-        <v>0.29194915254237286</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H47" s="11">
+        <f t="shared" si="2"/>
+        <v>0.10127118644067797</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>10</v>
       </c>
@@ -6607,12 +5946,12 @@
       <c r="F48" s="5">
         <v>0.19769999999999999</v>
       </c>
-      <c r="H48" s="12">
-        <f t="shared" si="0"/>
-        <v>0.3067020202020202</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H48" s="11">
+        <f t="shared" si="2"/>
+        <v>0.10889057239057238</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>10</v>
       </c>
@@ -6631,12 +5970,12 @@
       <c r="F49" s="5">
         <v>0.23499999999999999</v>
       </c>
-      <c r="H49" s="12">
-        <f t="shared" si="0"/>
-        <v>0.30924369747899161</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H49" s="11">
+        <f t="shared" si="2"/>
+        <v>0.10966386554621849</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>10</v>
       </c>
@@ -6655,12 +5994,12 @@
       <c r="F50" s="5">
         <v>0.25009999999999999</v>
       </c>
-      <c r="H50" s="12">
-        <f t="shared" si="0"/>
-        <v>0.31197913188647747</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H50" s="11">
+        <f>(F50*E50*8*A49+(100-E50)*10/96*96)/(E50*8*A49+(100-E50)*96)</f>
+        <v>0.10538480801335559</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>10</v>
       </c>
@@ -6679,12 +6018,12 @@
       <c r="F51" s="5">
         <v>0</v>
       </c>
-      <c r="H51" s="12">
-        <f t="shared" si="0"/>
+      <c r="H51" s="11">
+        <f t="shared" ref="H51:H57" si="3">(F51*E51*8*A50+(100-E51)*10/96*96)/(E51*8*A50+(100-E51)*96)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>10</v>
       </c>
@@ -6703,12 +6042,12 @@
       <c r="F52" s="5">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="H52" s="12">
-        <f t="shared" si="0"/>
-        <v>8.8053435114503822E-2</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H52" s="11">
+        <f t="shared" si="3"/>
+        <v>3.0801526717557252E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>10</v>
       </c>
@@ -6727,12 +6066,12 @@
       <c r="F53" s="5">
         <v>7.9000000000000008E-3</v>
       </c>
-      <c r="H53" s="12">
-        <f t="shared" si="0"/>
-        <v>0.13382402234636873</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H53" s="11">
+        <f t="shared" si="3"/>
+        <v>4.7697392923649912E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>10</v>
       </c>
@@ -6751,12 +6090,12 @@
       <c r="F54" s="5">
         <v>1.34E-2</v>
       </c>
-      <c r="H54" s="12">
-        <f t="shared" si="0"/>
-        <v>0.15246494464944649</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H54" s="11">
+        <f t="shared" si="3"/>
+        <v>5.5601476014760148E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>10</v>
       </c>
@@ -6775,12 +6114,12 @@
       <c r="F55" s="5">
         <v>1.8700000000000001E-2</v>
       </c>
-      <c r="H55" s="12">
-        <f t="shared" si="0"/>
-        <v>0.16425229357798166</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H55" s="11">
+        <f t="shared" si="3"/>
+        <v>6.1041284403669724E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>10</v>
       </c>
@@ -6799,12 +6138,12 @@
       <c r="F56" s="5">
         <v>3.2899999999999999E-2</v>
       </c>
-      <c r="H56" s="12">
-        <f t="shared" si="0"/>
-        <v>0.19642057761732851</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H56" s="11">
+        <f t="shared" si="3"/>
+        <v>7.4579422382671484E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>10</v>
       </c>
@@ -6823,12 +6162,12 @@
       <c r="F57" s="5">
         <v>0.20519999999999999</v>
       </c>
-      <c r="H57" s="12">
-        <f t="shared" si="0"/>
-        <v>0.28426315789473683</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H57" s="11">
+        <f t="shared" si="3"/>
+        <v>0.13075438596491229</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>10</v>
       </c>
@@ -6847,12 +6186,12 @@
       <c r="F58" s="5">
         <v>3.7100000000000001E-2</v>
       </c>
-      <c r="H58" s="12">
-        <f t="shared" si="0"/>
-        <v>0.26991237113402061</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H58" s="11">
+        <f>(F58*E58*8*A57+(100-E58)*10/96*96)/(E58*8*A57+(100-E58)*96)</f>
+        <v>9.3795532646048105E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>10</v>
       </c>
@@ -6871,12 +6210,12 @@
       <c r="F59" s="5">
         <v>4.9700000000000001E-2</v>
       </c>
-      <c r="H59" s="12">
-        <f t="shared" si="0"/>
-        <v>0.28110750853242322</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H59" s="11">
+        <f t="shared" ref="H59:H62" si="4">(F59*E59*8*A58+(100-E59)*10/96*96)/(E59*8*A58+(100-E59)*96)</f>
+        <v>9.7660409556313998E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>10</v>
       </c>
@@ -6895,12 +6234,12 @@
       <c r="F60" s="5">
         <v>7.4700000000000003E-2</v>
       </c>
-      <c r="H60" s="12">
-        <f t="shared" si="0"/>
-        <v>0.29846458684654298</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H60" s="11">
+        <f t="shared" si="4"/>
+        <v>0.1024274873524452</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>10</v>
       </c>
@@ -6919,12 +6258,12 @@
       <c r="F61" s="5">
         <v>8.2100000000000006E-2</v>
       </c>
-      <c r="H61" s="12">
-        <f t="shared" si="0"/>
-        <v>0.29297457627118645</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H61" s="11">
+        <f t="shared" si="4"/>
+        <v>0.10229661016949153</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>10</v>
       </c>
@@ -6943,9 +6282,9 @@
       <c r="F62" s="5">
         <v>0.43509999999999999</v>
       </c>
-      <c r="H62" s="12">
-        <f t="shared" si="0"/>
-        <v>0.31558040201005028</v>
+      <c r="H62" s="11">
+        <f t="shared" si="4"/>
+        <v>0.11248157453936349</v>
       </c>
     </row>
   </sheetData>
@@ -6975,16 +6314,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">

</xml_diff>